<commit_message>
Fix to cargo dist conversion factors
</commit_message>
<xml_diff>
--- a/InputData/web-app/CDCF/Cargo Dist Conversion Factors.xlsx
+++ b/InputData/web-app/CDCF/Cargo Dist Conversion Factors.xlsx
@@ -1,28 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\India InputData 5-6-2020\web-app\CDCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\web-app\CDCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2315D679-75BF-456D-9B52-FDDF8539BBEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF5ED90-C1E7-4BBA-9D82-B7C7731D523E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="CDCF-PMpPDOU" sheetId="2" r:id="rId2"/>
     <sheet name="CDCF-FTMpFDOU" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -563,7 +567,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,8 +586,8 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <f>1.60934*10^12</f>
-        <v>1609340000000</v>
+        <f>1/1.60934*10^12</f>
+        <v>621372736649.80676</v>
       </c>
     </row>
   </sheetData>
@@ -599,7 +603,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,8 +622,8 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <f>1.60934*10^12</f>
-        <v>1609340000000</v>
+        <f>1/1.60934*10^12</f>
+        <v>621372736649.80676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>